<commit_message>
api for spam classification using count vectorizer
</commit_message>
<xml_diff>
--- a/template/template_Sales_Agreement_v1.xlsx
+++ b/template/template_Sales_Agreement_v1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python_env\flask ml app\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53D9E0B-A0A9-494E-BA16-9F3E4AF1C4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E94A6E1-887C-4041-B0C2-5B8DF5667144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{6C8B0641-7AAF-469A-B417-9AD5EA3DD4FF}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7460" xr2:uid="{6C8B0641-7AAF-469A-B417-9AD5EA3DD4FF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sales Category" sheetId="1" r:id="rId1"/>
+    <sheet name="Config_Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -603,7 +603,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>

</xml_diff>